<commit_message>
Remove white space between analysis names
</commit_message>
<xml_diff>
--- a/tests/resources/metadata_2_analysis_same_samples.xlsx
+++ b/tests/resources/metadata_2_analysis_same_samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF84EE2A-A7FF-3541-AA82-F701DE04618B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2502AEE-547C-0942-8982-8455DE63EE8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42840" yWindow="1820" windowWidth="23260" windowHeight="12580" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="587">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -1789,6 +1789,9 @@
   </si>
   <si>
     <t>S1</t>
+  </si>
+  <si>
+    <t>GAE, GAE2</t>
   </si>
 </sst>
 </file>
@@ -2304,21 +2307,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2329,12 +2317,27 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2718,8 +2721,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="66"/>
-      <c r="B1" s="67"/>
+      <c r="A1" s="72"/>
+      <c r="B1" s="69"/>
       <c r="C1" s="63"/>
       <c r="D1" s="63"/>
       <c r="E1" s="63"/>
@@ -2728,10 +2731,10 @@
       <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="67"/>
+      <c r="B2" s="69"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -2740,10 +2743,10 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="67"/>
+      <c r="B3" s="69"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -2752,10 +2755,10 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="67"/>
+      <c r="B4" s="69"/>
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
       <c r="E4" s="62"/>
@@ -2764,8 +2767,8 @@
       <c r="H4" s="62"/>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="63"/>
       <c r="D5" s="63"/>
       <c r="E5" s="63"/>
@@ -2786,10 +2789,10 @@
       <c r="H6" s="62"/>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="67"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -2798,8 +2801,8 @@
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="74"/>
-      <c r="B8" s="67"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="63"/>
       <c r="D8" s="63"/>
       <c r="E8" s="63"/>
@@ -2808,10 +2811,10 @@
       <c r="H8" s="63"/>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="67"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="63"/>
       <c r="D9" s="63"/>
       <c r="E9" s="63"/>
@@ -2820,8 +2823,8 @@
       <c r="H9" s="63"/>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="66"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="72"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="63"/>
       <c r="D10" s="63"/>
       <c r="E10" s="63"/>
@@ -2830,10 +2833,10 @@
       <c r="H10" s="63"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="76"/>
+      <c r="B11" s="74"/>
     </row>
     <row r="12" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
@@ -2885,28 +2888,28 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="72"/>
+      <c r="B19" s="67"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="71" t="s">
+      <c r="A20" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="72"/>
+      <c r="B20" s="67"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="71" t="s">
+      <c r="A21" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="72"/>
+      <c r="B21" s="67"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="71" t="s">
+      <c r="A22" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="72"/>
+      <c r="B22" s="67"/>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
@@ -2915,6 +2918,11 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -2924,11 +2932,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5998,8 +6001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AMK102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6306,7 +6309,7 @@
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="F4" t="s">
         <v>585</v>
@@ -6426,7 +6429,7 @@
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A11" s="65" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="F11" t="s">
         <v>268</v>

</xml_diff>